<commit_message>
verify pagination test cases
</commit_message>
<xml_diff>
--- a/Excel/testdata.xlsx
+++ b/Excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rukhsaarhamid/PycharmProjects/ShiftERP/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EDF464-9481-FD42-85C3-026318AF0D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBDE15A-D2CC-CA4C-8C27-A2EDF52FE110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="4" xr2:uid="{87538411-8480-4141-BA9C-0C5B91401B4E}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="5" xr2:uid="{87538411-8480-4141-BA9C-0C5B91401B4E}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -18,26 +18,19 @@
     <sheet name="ManageAccounts-billingTest" sheetId="3" r:id="rId3"/>
     <sheet name="ManageAccounts-subTest" sheetId="4" r:id="rId4"/>
     <sheet name="ManageAccounts-settingsTest" sheetId="5" r:id="rId5"/>
+    <sheet name="ForgetPass" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>username</t>
   </si>
@@ -166,6 +159,18 @@
   </si>
   <si>
     <t>rukhsarhamid500+qa@gmail.com</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>rukhsarhamid500@gmail.com</t>
+  </si>
+  <si>
+    <t>wrongmail</t>
+  </si>
+  <si>
+    <t>rukhsarhamid@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -771,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECA0D70-F795-A545-A53C-021C31DE1881}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -824,4 +829,42 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C2F2771-5FCC-CB43-AC59-62A176FF01E0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{9818203E-DE06-324F-87F1-DCEC5DBB59DF}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{7FBE8C57-F3D9-744B-B14A-0962544D1D11}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>